<commit_message>
Fixed solution error calculation
Did it wrong before, but now it's good.
</commit_message>
<xml_diff>
--- a/MathProject/MathProject/Error Graphs.xlsx
+++ b/MathProject/MathProject/Error Graphs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben Bohannon\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben Bohannon\Documents\GitHub\Math-Project\MathProject\MathProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -707,11 +707,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="316229368"/>
-        <c:axId val="316232112"/>
+        <c:axId val="259859680"/>
+        <c:axId val="259861640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="316229368"/>
+        <c:axId val="259859680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -754,7 +754,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316232112"/>
+        <c:crossAx val="259861640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -762,7 +762,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="316232112"/>
+        <c:axId val="259861640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -813,7 +813,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316229368"/>
+        <c:crossAx val="259859680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1084,58 +1084,58 @@
                   <c:v>2.7755575615628901E-17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.3266726846886704E-17</c:v>
+                  <c:v>1.44222201478767E-16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5959455978986601E-16</c:v>
+                  <c:v>1.9279638981753101E-16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.7939764097625298E-16</c:v>
+                  <c:v>6.2238629252822901E-16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.7307270867900096E-16</c:v>
+                  <c:v>1.21122959637592E-15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.20576898360513E-15</c:v>
+                  <c:v>5.84146075820773E-15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.3635355585531796E-15</c:v>
+                  <c:v>1.39227653116285E-14</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.07618210817939E-14</c:v>
+                  <c:v>3.3090892498142802E-14</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.6275784813403197E-14</c:v>
+                  <c:v>1.01541403514341E-13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0706249797300099E-13</c:v>
+                  <c:v>1.67966473163536E-13</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.8753673162081E-13</c:v>
+                  <c:v>4.5397478097328498E-13</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.3905859986115599E-13</c:v>
+                  <c:v>8.5590848550735499E-13</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.8822650745460605E-13</c:v>
+                  <c:v>1.67749867022224E-12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.94584301485149E-14</c:v>
+                  <c:v>7.7551627198033899E-14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.5280542379136502E-13</c:v>
+                  <c:v>4.9903340384864197E-13</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.70482164592777E-14</c:v>
+                  <c:v>3.1799708363593902E-14</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.3002379117618699E-14</c:v>
+                  <c:v>9.0586057488778399E-14</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.3616131005177801E-15</c:v>
+                  <c:v>1.14186030700093E-14</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.8348513081212697E-15</c:v>
+                  <c:v>1.13971985490325E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1253,61 +1253,61 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>5.5511151231257802E-17</c:v>
+                  <c:v>7.8504622934188697E-17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4980018054066002E-16</c:v>
+                  <c:v>2.6477131637640601E-16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8449465006019602E-16</c:v>
+                  <c:v>4.1191555942998198E-16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0234868508263101E-15</c:v>
+                  <c:v>1.5112976233553601E-15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.3376079677793701E-15</c:v>
+                  <c:v>4.2516228637465597E-15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.98212582300539E-15</c:v>
+                  <c:v>7.1850897784420196E-15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.65054601930503E-14</c:v>
+                  <c:v>3.2829485749040401E-14</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.9174236691217302E-14</c:v>
+                  <c:v>1.02571519493975E-13</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.5688703591462599E-13</c:v>
+                  <c:v>2.1080826806222401E-13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.70487327197824E-13</c:v>
+                  <c:v>4.6978893112760297E-13</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.0691337409569199E-12</c:v>
+                  <c:v>1.77349252024219E-12</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.1271310007854404E-12</c:v>
+                  <c:v>1.47805373774055E-11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.80616292870758E-13</c:v>
+                  <c:v>4.9518169656751498E-13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.51864091513126E-13</c:v>
+                  <c:v>3.9359789122612201E-13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.2931560253832999E-13</c:v>
+                  <c:v>8.6730854858985803E-13</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.2229700277331901E-14</c:v>
+                  <c:v>1.3403243637673399E-13</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.38994834982432E-12</c:v>
+                  <c:v>5.5426682319679102E-12</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.8208229072675201E-14</c:v>
+                  <c:v>1.19519089375754E-13</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.9466728884211397E-15</c:v>
+                  <c:v>7.4326833910177798E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1428,58 +1428,58 @@
                   <c:v>1.94289029309402E-16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.3266726846886704E-17</c:v>
+                  <c:v>9.2054830157378606E-17</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.2450045135165006E-17</c:v>
+                  <c:v>1.2490009027033001E-16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.5286998857393398E-16</c:v>
+                  <c:v>7.7954543341933204E-16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.11716191852906E-15</c:v>
+                  <c:v>1.75022509210818E-15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.4523720527963601E-15</c:v>
+                  <c:v>1.0316331525006499E-14</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.7245319755554399E-14</c:v>
+                  <c:v>3.0237570586252699E-14</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.7857954618414303E-14</c:v>
+                  <c:v>6.9102685807164403E-14</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.63992463272227E-13</c:v>
+                  <c:v>2.3641843076100501E-13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.4206561776741999E-13</c:v>
+                  <c:v>4.1717783040100099E-13</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.2912126177924396E-13</c:v>
+                  <c:v>1.09837964101591E-12</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.5428253005100105E-11</c:v>
+                  <c:v>1.05919885043011E-10</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.9137060941612199E-13</c:v>
+                  <c:v>4.7467139625613101E-13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.1406541740332499E-13</c:v>
+                  <c:v>2.35122599135435E-13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.4622401342734999E-13</c:v>
+                  <c:v>2.7925982503291301E-13</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.6786207962484703E-14</c:v>
+                  <c:v>9.2326177993114396E-14</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.3579031246396202E-14</c:v>
+                  <c:v>1.05954409765209E-13</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.0444660678672703E-14</c:v>
+                  <c:v>5.8835229670622898E-14</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.2805390736460497E-15</c:v>
+                  <c:v>1.0079206560196301E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1496,11 +1496,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="323371960"/>
-        <c:axId val="323369216"/>
+        <c:axId val="259860072"/>
+        <c:axId val="259864384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="323371960"/>
+        <c:axId val="259860072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1543,7 +1543,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="323369216"/>
+        <c:crossAx val="259864384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1551,10 +1551,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="323369216"/>
+        <c:axId val="259864384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="4.0000000000000035E-15"/>
+          <c:max val="7.0000000000000065E-15"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1603,7 +1603,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="323371960"/>
+        <c:crossAx val="259860072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3126,8 +3126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:D44"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3439,7 +3439,7 @@
         <v>2.7755575615628901E-17</v>
       </c>
       <c r="C26" s="1">
-        <v>5.5511151231257802E-17</v>
+        <v>7.8504622934188697E-17</v>
       </c>
       <c r="D26" s="1">
         <v>1.94289029309402E-16</v>
@@ -3450,13 +3450,13 @@
         <v>3</v>
       </c>
       <c r="B27" s="1">
-        <v>8.3266726846886704E-17</v>
+        <v>1.44222201478767E-16</v>
       </c>
       <c r="C27" s="1">
-        <v>2.4980018054066002E-16</v>
+        <v>2.6477131637640601E-16</v>
       </c>
       <c r="D27" s="1">
-        <v>8.3266726846886704E-17</v>
+        <v>9.2054830157378606E-17</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3464,13 +3464,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1">
-        <v>1.5959455978986601E-16</v>
+        <v>1.9279638981753101E-16</v>
       </c>
       <c r="C28" s="1">
-        <v>2.8449465006019602E-16</v>
+        <v>4.1191555942998198E-16</v>
       </c>
       <c r="D28" s="1">
-        <v>6.2450045135165006E-17</v>
+        <v>1.2490009027033001E-16</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3478,13 +3478,13 @@
         <v>5</v>
       </c>
       <c r="B29" s="1">
-        <v>5.7939764097625298E-16</v>
+        <v>6.2238629252822901E-16</v>
       </c>
       <c r="C29" s="1">
-        <v>1.0234868508263101E-15</v>
+        <v>1.5112976233553601E-15</v>
       </c>
       <c r="D29" s="1">
-        <v>7.5286998857393398E-16</v>
+        <v>7.7954543341933204E-16</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3492,13 +3492,13 @@
         <v>6</v>
       </c>
       <c r="B30" s="1">
-        <v>6.7307270867900096E-16</v>
+        <v>1.21122959637592E-15</v>
       </c>
       <c r="C30" s="1">
-        <v>3.3376079677793701E-15</v>
+        <v>4.2516228637465597E-15</v>
       </c>
       <c r="D30" s="1">
-        <v>1.11716191852906E-15</v>
+        <v>1.75022509210818E-15</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3506,13 +3506,13 @@
         <v>7</v>
       </c>
       <c r="B31" s="1">
-        <v>3.20576898360513E-15</v>
+        <v>5.84146075820773E-15</v>
       </c>
       <c r="C31" s="1">
-        <v>4.98212582300539E-15</v>
+        <v>7.1850897784420196E-15</v>
       </c>
       <c r="D31" s="1">
-        <v>7.4523720527963601E-15</v>
+        <v>1.0316331525006499E-14</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3520,13 +3520,13 @@
         <v>8</v>
       </c>
       <c r="B32" s="1">
-        <v>8.3635355585531796E-15</v>
+        <v>1.39227653116285E-14</v>
       </c>
       <c r="C32" s="1">
-        <v>1.65054601930503E-14</v>
+        <v>3.2829485749040401E-14</v>
       </c>
       <c r="D32" s="1">
-        <v>1.7245319755554399E-14</v>
+        <v>3.0237570586252699E-14</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3534,13 +3534,13 @@
         <v>9</v>
       </c>
       <c r="B33" s="1">
-        <v>2.07618210817939E-14</v>
+        <v>3.3090892498142802E-14</v>
       </c>
       <c r="C33" s="1">
-        <v>5.9174236691217302E-14</v>
+        <v>1.02571519493975E-13</v>
       </c>
       <c r="D33" s="1">
-        <v>3.7857954618414303E-14</v>
+        <v>6.9102685807164403E-14</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3548,13 +3548,13 @@
         <v>10</v>
       </c>
       <c r="B34" s="1">
-        <v>5.6275784813403197E-14</v>
+        <v>1.01541403514341E-13</v>
       </c>
       <c r="C34" s="1">
-        <v>1.5688703591462599E-13</v>
+        <v>2.1080826806222401E-13</v>
       </c>
       <c r="D34" s="1">
-        <v>1.63992463272227E-13</v>
+        <v>2.3641843076100501E-13</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3562,13 +3562,13 @@
         <v>11</v>
       </c>
       <c r="B35" s="1">
-        <v>1.0706249797300099E-13</v>
+        <v>1.67966473163536E-13</v>
       </c>
       <c r="C35" s="1">
-        <v>2.70487327197824E-13</v>
+        <v>4.6978893112760297E-13</v>
       </c>
       <c r="D35" s="1">
-        <v>2.4206561776741999E-13</v>
+        <v>4.1717783040100099E-13</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3576,13 +3576,13 @@
         <v>12</v>
       </c>
       <c r="B36" s="1">
-        <v>2.8753673162081E-13</v>
+        <v>4.5397478097328498E-13</v>
       </c>
       <c r="C36" s="1">
-        <v>1.0691337409569199E-12</v>
+        <v>1.77349252024219E-12</v>
       </c>
       <c r="D36" s="1">
-        <v>5.2912126177924396E-13</v>
+        <v>1.09837964101591E-12</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -3590,13 +3590,13 @@
         <v>13</v>
       </c>
       <c r="B37" s="1">
-        <v>4.3905859986115599E-13</v>
+        <v>8.5590848550735499E-13</v>
       </c>
       <c r="C37" s="1">
-        <v>8.1271310007854404E-12</v>
+        <v>1.47805373774055E-11</v>
       </c>
       <c r="D37" s="1">
-        <v>6.5428253005100105E-11</v>
+        <v>1.05919885043011E-10</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -3604,13 +3604,13 @@
         <v>14</v>
       </c>
       <c r="B38" s="1">
-        <v>8.8822650745460605E-13</v>
+        <v>1.67749867022224E-12</v>
       </c>
       <c r="C38" s="1">
-        <v>2.80616292870758E-13</v>
+        <v>4.9518169656751498E-13</v>
       </c>
       <c r="D38" s="1">
-        <v>2.9137060941612199E-13</v>
+        <v>4.7467139625613101E-13</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3618,13 +3618,13 @@
         <v>15</v>
       </c>
       <c r="B39" s="1">
-        <v>3.94584301485149E-14</v>
+        <v>7.7551627198033899E-14</v>
       </c>
       <c r="C39" s="1">
-        <v>2.51864091513126E-13</v>
+        <v>3.9359789122612201E-13</v>
       </c>
       <c r="D39" s="1">
-        <v>1.1406541740332499E-13</v>
+        <v>2.35122599135435E-13</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3632,13 +3632,13 @@
         <v>16</v>
       </c>
       <c r="B40" s="1">
-        <v>2.5280542379136502E-13</v>
+        <v>4.9903340384864197E-13</v>
       </c>
       <c r="C40" s="1">
-        <v>4.2931560253832999E-13</v>
+        <v>8.6730854858985803E-13</v>
       </c>
       <c r="D40" s="1">
-        <v>1.4622401342734999E-13</v>
+        <v>2.7925982503291301E-13</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3646,13 +3646,13 @@
         <v>17</v>
       </c>
       <c r="B41" s="1">
-        <v>1.70482164592777E-14</v>
+        <v>3.1799708363593902E-14</v>
       </c>
       <c r="C41" s="1">
-        <v>5.2229700277331901E-14</v>
+        <v>1.3403243637673399E-13</v>
       </c>
       <c r="D41" s="1">
-        <v>6.6786207962484703E-14</v>
+        <v>9.2326177993114396E-14</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3660,13 +3660,13 @@
         <v>18</v>
       </c>
       <c r="B42" s="1">
-        <v>3.3002379117618699E-14</v>
+        <v>9.0586057488778399E-14</v>
       </c>
       <c r="C42" s="1">
-        <v>2.38994834982432E-12</v>
+        <v>5.5426682319679102E-12</v>
       </c>
       <c r="D42" s="1">
-        <v>7.3579031246396202E-14</v>
+        <v>1.05954409765209E-13</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3674,13 +3674,13 @@
         <v>19</v>
       </c>
       <c r="B43" s="1">
-        <v>5.3616131005177801E-15</v>
+        <v>1.14186030700093E-14</v>
       </c>
       <c r="C43" s="1">
-        <v>5.8208229072675201E-14</v>
+        <v>1.19519089375754E-13</v>
       </c>
       <c r="D43" s="1">
-        <v>4.0444660678672703E-14</v>
+        <v>5.8835229670622898E-14</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3688,13 +3688,13 @@
         <v>20</v>
       </c>
       <c r="B44" s="1">
-        <v>5.8348513081212697E-15</v>
+        <v>1.13971985490325E-14</v>
       </c>
       <c r="C44" s="1">
-        <v>4.9466728884211397E-15</v>
+        <v>7.4326833910177798E-15</v>
       </c>
       <c r="D44" s="1">
-        <v>4.2805390736460497E-15</v>
+        <v>1.0079206560196301E-14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>